<commit_message>
fix: Flipped Icon Font images
</commit_message>
<xml_diff>
--- a/src/ICON16x16.xlsx
+++ b/src/ICON16x16.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Data\work\Teensy40\VSCode\Mp3FilePlayer\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CBDB977-DEA7-49F9-836B-A1A46D7EE863}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{499AF711-153A-4D0E-83FC-1E0FC0EEC022}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4860" yWindow="240" windowWidth="28350" windowHeight="15135" xr2:uid="{7E682170-0FA3-4D33-A3CA-4458C6F2D2D4}"/>
+    <workbookView xWindow="150" yWindow="1065" windowWidth="28350" windowHeight="15150" xr2:uid="{7E682170-0FA3-4D33-A3CA-4458C6F2D2D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -514,7 +514,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94F949ED-4E88-4139-A003-24C46D6923AF}">
   <dimension ref="J12:AI135"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AI12" sqref="AI12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.125" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <sheetData>
@@ -536,16 +538,16 @@
       <c r="X12" s="3"/>
       <c r="Y12" s="4"/>
       <c r="AE12" t="str">
-        <f>DEC2HEX(R12*1+S12*2+T12*4+U12*8+V12*16+W12*32+X12*64+Y12*128, 2)</f>
+        <f>DEC2HEX(J12*128+K12*64+L12*32+M12*16+N12*8+O12*4+P12*2+Q12*1, 2)</f>
         <v>00</v>
       </c>
       <c r="AF12" t="str">
-        <f>DEC2HEX(J12*1+K12*2+L12*4+M12*8+N12*16+O12*32+P12*64+Q12*128, 2)</f>
+        <f>DEC2HEX(R12*128+S12*64+T12*32+U12*16+V12*8+W12*4+X12*2+Y12*1, 2)</f>
         <v>00</v>
       </c>
       <c r="AI12" t="str">
         <f>"0x"&amp;AE12&amp;",0x"&amp;AF12&amp;",0x"&amp;AE13&amp;",0x"&amp;AF13&amp;",0x"&amp;AE14&amp;",0x"&amp;AF14&amp;",0x"&amp;AE15&amp;",0x"&amp;AF15&amp;",0x"&amp;AE16&amp;",0x"&amp;AF16&amp;",0x"&amp;AE17&amp;",0x"&amp;AF17&amp;",0x"&amp;AE18&amp;",0x"&amp;AF18&amp;",0x"&amp;AE19&amp;",0x"&amp;AF19&amp;","</f>
-        <v>0x00,0x00,0x00,0x80,0x01,0x80,0x07,0x80,0x0F,0x80,0x1E,0x80,0x18,0x80,0x10,0x80,</v>
+        <v>0x00,0x00,0x01,0x00,0x01,0x80,0x01,0xE0,0x01,0xF0,0x01,0x78,0x01,0x18,0x01,0x08,</v>
       </c>
     </row>
     <row r="13" spans="10:35" x14ac:dyDescent="0.4">
@@ -567,16 +569,16 @@
       <c r="X13" s="1"/>
       <c r="Y13" s="6"/>
       <c r="AE13" t="str">
-        <f t="shared" ref="AE13:AE27" si="0">DEC2HEX(R13*1+S13*2+T13*4+U13*8+V13*16+W13*32+X13*64+Y13*128, 2)</f>
+        <f t="shared" ref="AE13:AE27" si="0">DEC2HEX(J13*128+K13*64+L13*32+M13*16+N13*8+O13*4+P13*2+Q13*1, 2)</f>
+        <v>01</v>
+      </c>
+      <c r="AF13" t="str">
+        <f t="shared" ref="AF13:AF27" si="1">DEC2HEX(R13*128+S13*64+T13*32+U13*16+V13*8+W13*4+X13*2+Y13*1, 2)</f>
         <v>00</v>
-      </c>
-      <c r="AF13" t="str">
-        <f t="shared" ref="AF13:AF27" si="1">DEC2HEX(J13*1+K13*2+L13*4+M13*8+N13*16+O13*32+P13*64+Q13*128, 2)</f>
-        <v>80</v>
       </c>
       <c r="AI13" t="str">
         <f>"0x"&amp;AE20&amp;",0x"&amp;AF20&amp;",0x"&amp;AE21&amp;",0x"&amp;AF21&amp;",0x"&amp;AE22&amp;",0x"&amp;AF22&amp;",0x"&amp;AE23&amp;",0x"&amp;AF23&amp;",0x"&amp;AE24&amp;",0x"&amp;AF24&amp;",0x"&amp;AE25&amp;",0x"&amp;AF25&amp;",0x"&amp;AE26&amp;",0x"&amp;AF26&amp;",0x"&amp;AE27&amp;",0x"&amp;AF27&amp;","</f>
-        <v>0x10,0x80,0x10,0x80,0x00,0xF0,0x00,0x78,0x00,0xFC,0x00,0x7C,0x00,0x38,0x00,0x00,</v>
+        <v>0x01,0x08,0x01,0x08,0x0F,0x00,0x1E,0x00,0x3F,0x00,0x3E,0x00,0x1C,0x00,0x00,0x00,</v>
       </c>
     </row>
     <row r="14" spans="10:35" x14ac:dyDescent="0.4">
@@ -636,11 +638,11 @@
       <c r="Y15" s="6"/>
       <c r="AE15" t="str">
         <f t="shared" si="0"/>
-        <v>07</v>
+        <v>01</v>
       </c>
       <c r="AF15" t="str">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>E0</v>
       </c>
     </row>
     <row r="16" spans="10:35" x14ac:dyDescent="0.4">
@@ -672,11 +674,11 @@
       <c r="Y16" s="6"/>
       <c r="AE16" t="str">
         <f t="shared" si="0"/>
-        <v>0F</v>
+        <v>01</v>
       </c>
       <c r="AF16" t="str">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>F0</v>
       </c>
     </row>
     <row r="17" spans="10:35" x14ac:dyDescent="0.4">
@@ -708,11 +710,11 @@
       <c r="Y17" s="6"/>
       <c r="AE17" t="str">
         <f t="shared" si="0"/>
-        <v>1E</v>
+        <v>01</v>
       </c>
       <c r="AF17" t="str">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="10:35" x14ac:dyDescent="0.4">
@@ -740,11 +742,11 @@
       <c r="Y18" s="6"/>
       <c r="AE18" t="str">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>01</v>
       </c>
       <c r="AF18" t="str">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="10:35" x14ac:dyDescent="0.4">
@@ -770,11 +772,11 @@
       <c r="Y19" s="6"/>
       <c r="AE19" t="str">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>01</v>
       </c>
       <c r="AF19" t="str">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>08</v>
       </c>
     </row>
     <row r="20" spans="10:35" x14ac:dyDescent="0.4">
@@ -800,11 +802,11 @@
       <c r="Y20" s="6"/>
       <c r="AE20" t="str">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>01</v>
       </c>
       <c r="AF20" t="str">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>08</v>
       </c>
     </row>
     <row r="21" spans="10:35" x14ac:dyDescent="0.4">
@@ -830,11 +832,11 @@
       <c r="Y21" s="6"/>
       <c r="AE21" t="str">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>01</v>
       </c>
       <c r="AF21" t="str">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>08</v>
       </c>
     </row>
     <row r="22" spans="10:35" x14ac:dyDescent="0.4">
@@ -864,11 +866,11 @@
       <c r="Y22" s="6"/>
       <c r="AE22" t="str">
         <f t="shared" si="0"/>
-        <v>00</v>
+        <v>0F</v>
       </c>
       <c r="AF22" t="str">
         <f t="shared" si="1"/>
-        <v>F0</v>
+        <v>00</v>
       </c>
     </row>
     <row r="23" spans="10:35" x14ac:dyDescent="0.4">
@@ -898,11 +900,11 @@
       <c r="Y23" s="6"/>
       <c r="AE23" t="str">
         <f t="shared" si="0"/>
-        <v>00</v>
+        <v>1E</v>
       </c>
       <c r="AF23" t="str">
         <f t="shared" si="1"/>
-        <v>78</v>
+        <v>00</v>
       </c>
     </row>
     <row r="24" spans="10:35" x14ac:dyDescent="0.4">
@@ -936,11 +938,11 @@
       <c r="Y24" s="6"/>
       <c r="AE24" t="str">
         <f t="shared" si="0"/>
-        <v>00</v>
+        <v>3F</v>
       </c>
       <c r="AF24" t="str">
         <f t="shared" si="1"/>
-        <v>FC</v>
+        <v>00</v>
       </c>
     </row>
     <row r="25" spans="10:35" x14ac:dyDescent="0.4">
@@ -972,11 +974,11 @@
       <c r="Y25" s="6"/>
       <c r="AE25" t="str">
         <f t="shared" si="0"/>
-        <v>00</v>
+        <v>3E</v>
       </c>
       <c r="AF25" t="str">
         <f t="shared" si="1"/>
-        <v>7C</v>
+        <v>00</v>
       </c>
     </row>
     <row r="26" spans="10:35" x14ac:dyDescent="0.4">
@@ -1004,11 +1006,11 @@
       <c r="Y26" s="6"/>
       <c r="AE26" t="str">
         <f t="shared" si="0"/>
-        <v>00</v>
+        <v>1C</v>
       </c>
       <c r="AF26" t="str">
         <f t="shared" si="1"/>
-        <v>38</v>
+        <v>00</v>
       </c>
     </row>
     <row r="27" spans="10:35" x14ac:dyDescent="0.4">
@@ -1055,16 +1057,16 @@
       <c r="X30" s="3"/>
       <c r="Y30" s="4"/>
       <c r="AE30" t="str">
-        <f>DEC2HEX(R30*1+S30*2+T30*4+U30*8+V30*16+W30*32+X30*64+Y30*128, 2)</f>
+        <f>DEC2HEX(J30*128+K30*64+L30*32+M30*16+N30*8+O30*4+P30*2+Q30*1, 2)</f>
         <v>00</v>
       </c>
       <c r="AF30" t="str">
-        <f>DEC2HEX(J30*1+K30*2+L30*4+M30*8+N30*16+O30*32+P30*64+Q30*128, 2)</f>
+        <f>DEC2HEX(R30*128+S30*64+T30*32+U30*16+V30*8+W30*4+X30*2+Y30*1, 2)</f>
         <v>00</v>
       </c>
       <c r="AI30" t="str">
         <f>"0x"&amp;AE30&amp;",0x"&amp;AF30&amp;",0x"&amp;AE31&amp;",0x"&amp;AF31&amp;",0x"&amp;AE32&amp;",0x"&amp;AF32&amp;",0x"&amp;AE33&amp;",0x"&amp;AF33&amp;",0x"&amp;AE34&amp;",0x"&amp;AF34&amp;",0x"&amp;AE35&amp;",0x"&amp;AF35&amp;",0x"&amp;AE36&amp;",0x"&amp;AF36&amp;",0x"&amp;AE37&amp;",0x"&amp;AF37&amp;","</f>
-        <v>0x00,0x00,0x01,0xF0,0x07,0xF8,0x0F,0xFC,0x1E,0xAC,0x1C,0x06,0x39,0x12,0x38,0x42,</v>
+        <v>0x00,0x00,0x0F,0x80,0x1F,0xE0,0x3F,0xF0,0x35,0x78,0x60,0x38,0x48,0x9C,0x42,0x1C,</v>
       </c>
     </row>
     <row r="31" spans="10:35" x14ac:dyDescent="0.4">
@@ -1095,16 +1097,16 @@
       <c r="X31" s="1"/>
       <c r="Y31" s="6"/>
       <c r="AE31" t="str">
-        <f t="shared" ref="AE31:AE45" si="2">DEC2HEX(R31*1+S31*2+T31*4+U31*8+V31*16+W31*32+X31*64+Y31*128, 2)</f>
-        <v>01</v>
+        <f t="shared" ref="AE31:AE45" si="2">DEC2HEX(J31*128+K31*64+L31*32+M31*16+N31*8+O31*4+P31*2+Q31*1, 2)</f>
+        <v>0F</v>
       </c>
       <c r="AF31" t="str">
-        <f t="shared" ref="AF31:AF45" si="3">DEC2HEX(J31*1+K31*2+L31*4+M31*8+N31*16+O31*32+P31*64+Q31*128, 2)</f>
-        <v>F0</v>
+        <f t="shared" ref="AF31:AF45" si="3">DEC2HEX(R31*128+S31*64+T31*32+U31*16+V31*8+W31*4+X31*2+Y31*1, 2)</f>
+        <v>80</v>
       </c>
       <c r="AI31" t="str">
         <f>"0x"&amp;AE38&amp;",0x"&amp;AF38&amp;",0x"&amp;AE39&amp;",0x"&amp;AF39&amp;",0x"&amp;AE40&amp;",0x"&amp;AF40&amp;",0x"&amp;AE41&amp;",0x"&amp;AF41&amp;",0x"&amp;AE42&amp;",0x"&amp;AF42&amp;",0x"&amp;AE43&amp;",0x"&amp;AF43&amp;",0x"&amp;AE44&amp;",0x"&amp;AF44&amp;",0x"&amp;AE45&amp;",0x"&amp;AF45&amp;","</f>
-        <v>0x78,0x02,0x7C,0x84,0x7C,0xE4,0x3A,0x08,0x71,0x10,0x27,0x1C,0x0B,0xFA,0x00,0x00,</v>
+        <v>0x40,0x1E,0x21,0x3E,0x27,0x3E,0x10,0x5C,0x08,0x8E,0x38,0xE4,0x5F,0xD0,0x00,0x00,</v>
       </c>
     </row>
     <row r="32" spans="10:35" x14ac:dyDescent="0.4">
@@ -1142,11 +1144,11 @@
       <c r="Y32" s="6"/>
       <c r="AE32" t="str">
         <f t="shared" si="2"/>
-        <v>07</v>
+        <v>1F</v>
       </c>
       <c r="AF32" t="str">
         <f t="shared" si="3"/>
-        <v>F8</v>
+        <v>E0</v>
       </c>
     </row>
     <row r="33" spans="10:35" x14ac:dyDescent="0.4">
@@ -1188,11 +1190,11 @@
       <c r="Y33" s="6"/>
       <c r="AE33" t="str">
         <f t="shared" si="2"/>
-        <v>0F</v>
+        <v>3F</v>
       </c>
       <c r="AF33" t="str">
         <f t="shared" si="3"/>
-        <v>FC</v>
+        <v>F0</v>
       </c>
     </row>
     <row r="34" spans="10:35" x14ac:dyDescent="0.4">
@@ -1230,11 +1232,11 @@
       <c r="Y34" s="6"/>
       <c r="AE34" t="str">
         <f t="shared" si="2"/>
-        <v>1E</v>
+        <v>35</v>
       </c>
       <c r="AF34" t="str">
         <f t="shared" si="3"/>
-        <v>AC</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35" spans="10:35" x14ac:dyDescent="0.4">
@@ -1266,11 +1268,11 @@
       <c r="Y35" s="6"/>
       <c r="AE35" t="str">
         <f t="shared" si="2"/>
-        <v>1C</v>
+        <v>60</v>
       </c>
       <c r="AF35" t="str">
         <f t="shared" si="3"/>
-        <v>06</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="10:35" x14ac:dyDescent="0.4">
@@ -1304,11 +1306,11 @@
       <c r="Y36" s="6"/>
       <c r="AE36" t="str">
         <f t="shared" si="2"/>
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="AF36" t="str">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>9C</v>
       </c>
     </row>
     <row r="37" spans="10:35" x14ac:dyDescent="0.4">
@@ -1340,11 +1342,11 @@
       <c r="Y37" s="6"/>
       <c r="AE37" t="str">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="AF37" t="str">
         <f t="shared" si="3"/>
-        <v>42</v>
+        <v>1C</v>
       </c>
     </row>
     <row r="38" spans="10:35" x14ac:dyDescent="0.4">
@@ -1376,11 +1378,11 @@
       <c r="Y38" s="6"/>
       <c r="AE38" t="str">
         <f t="shared" si="2"/>
-        <v>78</v>
+        <v>40</v>
       </c>
       <c r="AF38" t="str">
         <f t="shared" si="3"/>
-        <v>02</v>
+        <v>1E</v>
       </c>
     </row>
     <row r="39" spans="10:35" x14ac:dyDescent="0.4">
@@ -1416,11 +1418,11 @@
       <c r="Y39" s="6"/>
       <c r="AE39" t="str">
         <f t="shared" si="2"/>
-        <v>7C</v>
+        <v>21</v>
       </c>
       <c r="AF39" t="str">
         <f t="shared" si="3"/>
-        <v>84</v>
+        <v>3E</v>
       </c>
     </row>
     <row r="40" spans="10:35" x14ac:dyDescent="0.4">
@@ -1459,11 +1461,11 @@
       <c r="Y40" s="6"/>
       <c r="AE40" t="str">
         <f t="shared" si="2"/>
-        <v>7C</v>
+        <v>27</v>
       </c>
       <c r="AF40" t="str">
         <f t="shared" si="3"/>
-        <v>E4</v>
+        <v>3E</v>
       </c>
     </row>
     <row r="41" spans="10:35" x14ac:dyDescent="0.4">
@@ -1495,11 +1497,11 @@
       <c r="Y41" s="6"/>
       <c r="AE41" t="str">
         <f t="shared" si="2"/>
-        <v>3A</v>
+        <v>10</v>
       </c>
       <c r="AF41" t="str">
         <f t="shared" si="3"/>
-        <v>08</v>
+        <v>5C</v>
       </c>
     </row>
     <row r="42" spans="10:35" x14ac:dyDescent="0.4">
@@ -1531,11 +1533,11 @@
       <c r="Y42" s="6"/>
       <c r="AE42" t="str">
         <f t="shared" si="2"/>
-        <v>71</v>
+        <v>08</v>
       </c>
       <c r="AF42" t="str">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>8E</v>
       </c>
     </row>
     <row r="43" spans="10:35" x14ac:dyDescent="0.4">
@@ -1571,11 +1573,11 @@
       <c r="Y43" s="6"/>
       <c r="AE43" t="str">
         <f t="shared" si="2"/>
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="AF43" t="str">
         <f t="shared" si="3"/>
-        <v>1C</v>
+        <v>E4</v>
       </c>
     </row>
     <row r="44" spans="10:35" x14ac:dyDescent="0.4">
@@ -1615,11 +1617,11 @@
       <c r="Y44" s="6"/>
       <c r="AE44" t="str">
         <f t="shared" si="2"/>
-        <v>0B</v>
+        <v>5F</v>
       </c>
       <c r="AF44" t="str">
         <f t="shared" si="3"/>
-        <v>FA</v>
+        <v>D0</v>
       </c>
     </row>
     <row r="45" spans="10:35" x14ac:dyDescent="0.4">
@@ -1666,16 +1668,16 @@
       <c r="X48" s="3"/>
       <c r="Y48" s="4"/>
       <c r="AE48" t="str">
-        <f>DEC2HEX(R48*1+S48*2+T48*4+U48*8+V48*16+W48*32+X48*64+Y48*128, 2)</f>
+        <f>DEC2HEX(J48*128+K48*64+L48*32+M48*16+N48*8+O48*4+P48*2+Q48*1, 2)</f>
         <v>00</v>
       </c>
       <c r="AF48" t="str">
-        <f>DEC2HEX(J48*1+K48*2+L48*4+M48*8+N48*16+O48*32+P48*64+Q48*128, 2)</f>
+        <f>DEC2HEX(R48*128+S48*64+T48*32+U48*16+V48*8+W48*4+X48*2+Y48*1, 2)</f>
         <v>00</v>
       </c>
       <c r="AI48" t="str">
         <f>"0x"&amp;AE48&amp;",0x"&amp;AF48&amp;",0x"&amp;AE49&amp;",0x"&amp;AF49&amp;",0x"&amp;AE50&amp;",0x"&amp;AF50&amp;",0x"&amp;AE51&amp;",0x"&amp;AF51&amp;",0x"&amp;AE52&amp;",0x"&amp;AF52&amp;",0x"&amp;AE53&amp;",0x"&amp;AF53&amp;",0x"&amp;AE54&amp;",0x"&amp;AF54&amp;",0x"&amp;AE55&amp;",0x"&amp;AF55&amp;","</f>
-        <v>0x00,0x00,0x0F,0x00,0x08,0xE0,0x08,0x18,0x3F,0xFE,0x20,0x02,0x20,0x82,0x21,0x42,</v>
+        <v>0x00,0x00,0x00,0xF0,0x07,0x10,0x18,0x10,0x7F,0xFC,0x40,0x04,0x41,0x04,0x42,0x84,</v>
       </c>
     </row>
     <row r="49" spans="10:35" x14ac:dyDescent="0.4">
@@ -1704,16 +1706,16 @@
       <c r="X49" s="1"/>
       <c r="Y49" s="6"/>
       <c r="AE49" t="str">
-        <f t="shared" ref="AE49:AE63" si="4">DEC2HEX(R49*1+S49*2+T49*4+U49*8+V49*16+W49*32+X49*64+Y49*128, 2)</f>
-        <v>0F</v>
+        <f t="shared" ref="AE49:AE63" si="4">DEC2HEX(J49*128+K49*64+L49*32+M49*16+N49*8+O49*4+P49*2+Q49*1, 2)</f>
+        <v>00</v>
       </c>
       <c r="AF49" t="str">
-        <f t="shared" ref="AF49:AF63" si="5">DEC2HEX(J49*1+K49*2+L49*4+M49*8+N49*16+O49*32+P49*64+Q49*128, 2)</f>
-        <v>00</v>
+        <f t="shared" ref="AF49:AF63" si="5">DEC2HEX(R49*128+S49*64+T49*32+U49*16+V49*8+W49*4+X49*2+Y49*1, 2)</f>
+        <v>F0</v>
       </c>
       <c r="AI49" t="str">
         <f>"0x"&amp;AE56&amp;",0x"&amp;AF56&amp;",0x"&amp;AE57&amp;",0x"&amp;AF57&amp;",0x"&amp;AE58&amp;",0x"&amp;AF58&amp;",0x"&amp;AE59&amp;",0x"&amp;AF59&amp;",0x"&amp;AE60&amp;",0x"&amp;AF60&amp;",0x"&amp;AE61&amp;",0x"&amp;AF61&amp;",0x"&amp;AE62&amp;",0x"&amp;AF62&amp;",0x"&amp;AE63&amp;",0x"&amp;AF63&amp;","</f>
-        <v>0x26,0x72,0x2A,0x2A,0x34,0x16,0x27,0xF2,0x20,0x02,0x20,0x02,0x3F,0xFE,0x00,0x00,</v>
+        <v>0x4E,0x64,0x54,0x54,0x68,0x2C,0x4F,0xE4,0x40,0x04,0x40,0x04,0x7F,0xFC,0x00,0x00,</v>
       </c>
     </row>
     <row r="50" spans="10:35" x14ac:dyDescent="0.4">
@@ -1743,11 +1745,11 @@
       <c r="Y50" s="6"/>
       <c r="AE50" t="str">
         <f t="shared" si="4"/>
-        <v>08</v>
+        <v>07</v>
       </c>
       <c r="AF50" t="str">
         <f t="shared" si="5"/>
-        <v>E0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="10:35" x14ac:dyDescent="0.4">
@@ -1775,11 +1777,11 @@
       <c r="Y51" s="6"/>
       <c r="AE51" t="str">
         <f t="shared" si="4"/>
-        <v>08</v>
+        <v>18</v>
       </c>
       <c r="AF51" t="str">
         <f t="shared" si="5"/>
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="52" spans="10:35" x14ac:dyDescent="0.4">
@@ -1827,11 +1829,11 @@
       <c r="Y52" s="6"/>
       <c r="AE52" t="str">
         <f t="shared" si="4"/>
-        <v>3F</v>
+        <v>7F</v>
       </c>
       <c r="AF52" t="str">
         <f t="shared" si="5"/>
-        <v>FE</v>
+        <v>FC</v>
       </c>
     </row>
     <row r="53" spans="10:35" x14ac:dyDescent="0.4">
@@ -1857,11 +1859,11 @@
       <c r="Y53" s="6"/>
       <c r="AE53" t="str">
         <f t="shared" si="4"/>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="AF53" t="str">
         <f t="shared" si="5"/>
-        <v>02</v>
+        <v>04</v>
       </c>
     </row>
     <row r="54" spans="10:35" x14ac:dyDescent="0.4">
@@ -1889,11 +1891,11 @@
       <c r="Y54" s="6"/>
       <c r="AE54" t="str">
         <f t="shared" si="4"/>
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="AF54" t="str">
         <f t="shared" si="5"/>
-        <v>82</v>
+        <v>04</v>
       </c>
     </row>
     <row r="55" spans="10:35" x14ac:dyDescent="0.4">
@@ -1922,11 +1924,11 @@
       <c r="Y55" s="6"/>
       <c r="AE55" t="str">
         <f t="shared" si="4"/>
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="AF55" t="str">
         <f t="shared" si="5"/>
-        <v>42</v>
+        <v>84</v>
       </c>
     </row>
     <row r="56" spans="10:35" x14ac:dyDescent="0.4">
@@ -1962,11 +1964,11 @@
       <c r="Y56" s="6"/>
       <c r="AE56" t="str">
         <f t="shared" si="4"/>
-        <v>26</v>
+        <v>4E</v>
       </c>
       <c r="AF56" t="str">
         <f t="shared" si="5"/>
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="57" spans="10:35" x14ac:dyDescent="0.4">
@@ -2000,11 +2002,11 @@
       <c r="Y57" s="6"/>
       <c r="AE57" t="str">
         <f t="shared" si="4"/>
-        <v>2A</v>
+        <v>54</v>
       </c>
       <c r="AF57" t="str">
         <f t="shared" si="5"/>
-        <v>2A</v>
+        <v>54</v>
       </c>
     </row>
     <row r="58" spans="10:35" x14ac:dyDescent="0.4">
@@ -2038,11 +2040,11 @@
       <c r="Y58" s="6"/>
       <c r="AE58" t="str">
         <f t="shared" si="4"/>
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="AF58" t="str">
         <f t="shared" si="5"/>
-        <v>16</v>
+        <v>2C</v>
       </c>
     </row>
     <row r="59" spans="10:35" x14ac:dyDescent="0.4">
@@ -2082,11 +2084,11 @@
       <c r="Y59" s="6"/>
       <c r="AE59" t="str">
         <f t="shared" si="4"/>
-        <v>27</v>
+        <v>4F</v>
       </c>
       <c r="AF59" t="str">
         <f t="shared" si="5"/>
-        <v>F2</v>
+        <v>E4</v>
       </c>
     </row>
     <row r="60" spans="10:35" x14ac:dyDescent="0.4">
@@ -2112,11 +2114,11 @@
       <c r="Y60" s="6"/>
       <c r="AE60" t="str">
         <f t="shared" si="4"/>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="AF60" t="str">
         <f t="shared" si="5"/>
-        <v>02</v>
+        <v>04</v>
       </c>
     </row>
     <row r="61" spans="10:35" x14ac:dyDescent="0.4">
@@ -2142,11 +2144,11 @@
       <c r="Y61" s="6"/>
       <c r="AE61" t="str">
         <f t="shared" si="4"/>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="AF61" t="str">
         <f t="shared" si="5"/>
-        <v>02</v>
+        <v>04</v>
       </c>
     </row>
     <row r="62" spans="10:35" x14ac:dyDescent="0.4">
@@ -2194,11 +2196,11 @@
       <c r="Y62" s="6"/>
       <c r="AE62" t="str">
         <f t="shared" si="4"/>
-        <v>3F</v>
+        <v>7F</v>
       </c>
       <c r="AF62" t="str">
         <f t="shared" si="5"/>
-        <v>FE</v>
+        <v>FC</v>
       </c>
     </row>
     <row r="63" spans="10:35" x14ac:dyDescent="0.4">
@@ -2245,16 +2247,16 @@
       <c r="X66" s="3"/>
       <c r="Y66" s="4"/>
       <c r="AE66" t="str">
-        <f>DEC2HEX(R66*1+S66*2+T66*4+U66*8+V66*16+W66*32+X66*64+Y66*128, 2)</f>
+        <f>DEC2HEX(J66*128+K66*64+L66*32+M66*16+N66*8+O66*4+P66*2+Q66*1, 2)</f>
         <v>00</v>
       </c>
       <c r="AF66" t="str">
-        <f>DEC2HEX(J66*1+K66*2+L66*4+M66*8+N66*16+O66*32+P66*64+Q66*128, 2)</f>
+        <f>DEC2HEX(R66*128+S66*64+T66*32+U66*16+V66*8+W66*4+X66*2+Y66*1, 2)</f>
         <v>00</v>
       </c>
       <c r="AI66" t="str">
         <f>"0x"&amp;AE66&amp;",0x"&amp;AF66&amp;",0x"&amp;AE67&amp;",0x"&amp;AF67&amp;",0x"&amp;AE68&amp;",0x"&amp;AF68&amp;",0x"&amp;AE69&amp;",0x"&amp;AF69&amp;",0x"&amp;AE70&amp;",0x"&amp;AF70&amp;",0x"&amp;AE71&amp;",0x"&amp;AF71&amp;",0x"&amp;AE72&amp;",0x"&amp;AF72&amp;",0x"&amp;AE73&amp;",0x"&amp;AF73&amp;","</f>
-        <v>0x00,0x00,0x00,0xFC,0x01,0x86,0x03,0x02,0x3E,0x02,0x60,0x02,0x40,0x02,0x40,0x02,</v>
+        <v>0x00,0x00,0x3F,0x00,0x61,0x80,0x40,0xC0,0x40,0x7C,0x40,0x06,0x40,0x02,0x40,0x02,</v>
       </c>
     </row>
     <row r="67" spans="10:35" x14ac:dyDescent="0.4">
@@ -2287,12 +2289,12 @@
       <c r="X67" s="1"/>
       <c r="Y67" s="6"/>
       <c r="AE67" t="str">
-        <f t="shared" ref="AE67:AE81" si="6">DEC2HEX(R67*1+S67*2+T67*4+U67*8+V67*16+W67*32+X67*64+Y67*128, 2)</f>
+        <f t="shared" ref="AE67:AE81" si="6">DEC2HEX(J67*128+K67*64+L67*32+M67*16+N67*8+O67*4+P67*2+Q67*1, 2)</f>
+        <v>3F</v>
+      </c>
+      <c r="AF67" t="str">
+        <f t="shared" ref="AF67:AF81" si="7">DEC2HEX(R67*128+S67*64+T67*32+U67*16+V67*8+W67*4+X67*2+Y67*1, 2)</f>
         <v>00</v>
-      </c>
-      <c r="AF67" t="str">
-        <f t="shared" ref="AF67:AF81" si="7">DEC2HEX(J67*1+K67*2+L67*4+M67*8+N67*16+O67*32+P67*64+Q67*128, 2)</f>
-        <v>FC</v>
       </c>
       <c r="AI67" t="str">
         <f>"0x"&amp;AE74&amp;",0x"&amp;AF74&amp;",0x"&amp;AE75&amp;",0x"&amp;AF75&amp;",0x"&amp;AE76&amp;",0x"&amp;AF76&amp;",0x"&amp;AE77&amp;",0x"&amp;AF77&amp;",0x"&amp;AE78&amp;",0x"&amp;AF78&amp;",0x"&amp;AE79&amp;",0x"&amp;AF79&amp;",0x"&amp;AE80&amp;",0x"&amp;AF80&amp;",0x"&amp;AE81&amp;",0x"&amp;AF81&amp;","</f>
@@ -2326,11 +2328,11 @@
       <c r="Y68" s="6"/>
       <c r="AE68" t="str">
         <f t="shared" si="6"/>
-        <v>01</v>
+        <v>61</v>
       </c>
       <c r="AF68" t="str">
         <f t="shared" si="7"/>
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="69" spans="10:35" x14ac:dyDescent="0.4">
@@ -2358,11 +2360,11 @@
       <c r="Y69" s="6"/>
       <c r="AE69" t="str">
         <f t="shared" si="6"/>
-        <v>03</v>
+        <v>40</v>
       </c>
       <c r="AF69" t="str">
         <f t="shared" si="7"/>
-        <v>02</v>
+        <v>C0</v>
       </c>
     </row>
     <row r="70" spans="10:35" x14ac:dyDescent="0.4">
@@ -2396,11 +2398,11 @@
       <c r="Y70" s="6"/>
       <c r="AE70" t="str">
         <f t="shared" si="6"/>
-        <v>3E</v>
+        <v>40</v>
       </c>
       <c r="AF70" t="str">
         <f t="shared" si="7"/>
-        <v>02</v>
+        <v>7C</v>
       </c>
     </row>
     <row r="71" spans="10:35" x14ac:dyDescent="0.4">
@@ -2428,11 +2430,11 @@
       <c r="Y71" s="6"/>
       <c r="AE71" t="str">
         <f t="shared" si="6"/>
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="AF71" t="str">
         <f t="shared" si="7"/>
-        <v>02</v>
+        <v>06</v>
       </c>
     </row>
     <row r="72" spans="10:35" x14ac:dyDescent="0.4">
@@ -2773,11 +2775,11 @@
       <c r="X84" s="3"/>
       <c r="Y84" s="4"/>
       <c r="AE84" t="str">
-        <f>DEC2HEX(R84*1+S84*2+T84*4+U84*8+V84*16+W84*32+X84*64+Y84*128, 2)</f>
+        <f>DEC2HEX(J84*128+K84*64+L84*32+M84*16+N84*8+O84*4+P84*2+Q84*1, 2)</f>
         <v>00</v>
       </c>
       <c r="AF84" t="str">
-        <f>DEC2HEX(J84*1+K84*2+L84*4+M84*8+N84*16+O84*32+P84*64+Q84*128, 2)</f>
+        <f>DEC2HEX(R84*128+S84*64+T84*32+U84*16+V84*8+W84*4+X84*2+Y84*1, 2)</f>
         <v>00</v>
       </c>
       <c r="AI84" t="str">
@@ -2803,11 +2805,11 @@
       <c r="X85" s="1"/>
       <c r="Y85" s="6"/>
       <c r="AE85" t="str">
-        <f t="shared" ref="AE85:AE99" si="8">DEC2HEX(R85*1+S85*2+T85*4+U85*8+V85*16+W85*32+X85*64+Y85*128, 2)</f>
+        <f t="shared" ref="AE85:AE99" si="8">DEC2HEX(J85*128+K85*64+L85*32+M85*16+N85*8+O85*4+P85*2+Q85*1, 2)</f>
         <v>00</v>
       </c>
       <c r="AF85" t="str">
-        <f t="shared" ref="AF85:AF99" si="9">DEC2HEX(J85*1+K85*2+L85*4+M85*8+N85*16+O85*32+P85*64+Q85*128, 2)</f>
+        <f t="shared" ref="AF85:AF99" si="9">DEC2HEX(R85*128+S85*64+T85*32+U85*16+V85*8+W85*4+X85*2+Y85*1, 2)</f>
         <v>00</v>
       </c>
       <c r="AI85" t="str">
@@ -3325,16 +3327,16 @@
       <c r="X102" s="3"/>
       <c r="Y102" s="4"/>
       <c r="AE102" t="str">
-        <f>DEC2HEX(R102*1+S102*2+T102*4+U102*8+V102*16+W102*32+X102*64+Y102*128, 2)</f>
+        <f>DEC2HEX(J102*128+K102*64+L102*32+M102*16+N102*8+O102*4+P102*2+Q102*1, 2)</f>
         <v>00</v>
       </c>
       <c r="AF102" t="str">
-        <f>DEC2HEX(J102*1+K102*2+L102*4+M102*8+N102*16+O102*32+P102*64+Q102*128, 2)</f>
+        <f>DEC2HEX(R102*128+S102*64+T102*32+U102*16+V102*8+W102*4+X102*2+Y102*1, 2)</f>
         <v>00</v>
       </c>
       <c r="AI102" t="str">
         <f>"0x"&amp;AE102&amp;",0x"&amp;AF102&amp;",0x"&amp;AE103&amp;",0x"&amp;AF103&amp;",0x"&amp;AE104&amp;",0x"&amp;AF104&amp;",0x"&amp;AE105&amp;",0x"&amp;AF105&amp;",0x"&amp;AE106&amp;",0x"&amp;AF106&amp;",0x"&amp;AE107&amp;",0x"&amp;AF107&amp;",0x"&amp;AE108&amp;",0x"&amp;AF108&amp;",0x"&amp;AE109&amp;",0x"&amp;AF109&amp;","</f>
-        <v>0x00,0x00,0x00,0x00,0x1E,0x00,0x13,0x00,0x11,0x80,0x10,0xC0,0x10,0x78,0x10,0x48,</v>
+        <v>0x00,0x00,0x00,0x00,0x00,0x78,0x00,0xC8,0x01,0x88,0x03,0x08,0x1E,0x08,0x12,0x08,</v>
       </c>
     </row>
     <row r="103" spans="10:35" x14ac:dyDescent="0.4">
@@ -3355,16 +3357,16 @@
       <c r="X103" s="1"/>
       <c r="Y103" s="6"/>
       <c r="AE103" t="str">
-        <f t="shared" ref="AE103:AE117" si="10">DEC2HEX(R103*1+S103*2+T103*4+U103*8+V103*16+W103*32+X103*64+Y103*128, 2)</f>
+        <f t="shared" ref="AE103:AE117" si="10">DEC2HEX(J103*128+K103*64+L103*32+M103*16+N103*8+O103*4+P103*2+Q103*1, 2)</f>
         <v>00</v>
       </c>
       <c r="AF103" t="str">
-        <f t="shared" ref="AF103:AF117" si="11">DEC2HEX(J103*1+K103*2+L103*4+M103*8+N103*16+O103*32+P103*64+Q103*128, 2)</f>
+        <f t="shared" ref="AF103:AF117" si="11">DEC2HEX(R103*128+S103*64+T103*32+U103*16+V103*8+W103*4+X103*2+Y103*1, 2)</f>
         <v>00</v>
       </c>
       <c r="AI103" t="str">
         <f>"0x"&amp;AE110&amp;",0x"&amp;AF110&amp;",0x"&amp;AE111&amp;",0x"&amp;AF111&amp;",0x"&amp;AE112&amp;",0x"&amp;AF112&amp;",0x"&amp;AE113&amp;",0x"&amp;AF113&amp;",0x"&amp;AE114&amp;",0x"&amp;AF114&amp;",0x"&amp;AE115&amp;",0x"&amp;AF115&amp;",0x"&amp;AE116&amp;",0x"&amp;AF116&amp;",0x"&amp;AE117&amp;",0x"&amp;AF117&amp;","</f>
-        <v>0x10,0x48,0x10,0x48,0x10,0x78,0x10,0xC0,0x11,0x80,0x13,0x00,0x1E,0x00,0x00,0x00,</v>
+        <v>0x12,0x08,0x12,0x08,0x1E,0x08,0x03,0x08,0x01,0x88,0x00,0xC8,0x00,0x78,0x00,0x00,</v>
       </c>
     </row>
     <row r="104" spans="10:35" x14ac:dyDescent="0.4">
@@ -3394,11 +3396,11 @@
       <c r="Y104" s="6"/>
       <c r="AE104" t="str">
         <f t="shared" si="10"/>
-        <v>1E</v>
+        <v>00</v>
       </c>
       <c r="AF104" t="str">
         <f t="shared" si="11"/>
-        <v>00</v>
+        <v>78</v>
       </c>
     </row>
     <row r="105" spans="10:35" x14ac:dyDescent="0.4">
@@ -3426,11 +3428,11 @@
       <c r="Y105" s="6"/>
       <c r="AE105" t="str">
         <f t="shared" si="10"/>
-        <v>13</v>
+        <v>00</v>
       </c>
       <c r="AF105" t="str">
         <f t="shared" si="11"/>
-        <v>00</v>
+        <v>C8</v>
       </c>
     </row>
     <row r="106" spans="10:35" x14ac:dyDescent="0.4">
@@ -3458,11 +3460,11 @@
       <c r="Y106" s="6"/>
       <c r="AE106" t="str">
         <f t="shared" si="10"/>
-        <v>11</v>
+        <v>01</v>
       </c>
       <c r="AF106" t="str">
         <f t="shared" si="11"/>
-        <v>80</v>
+        <v>88</v>
       </c>
     </row>
     <row r="107" spans="10:35" x14ac:dyDescent="0.4">
@@ -3490,11 +3492,11 @@
       <c r="Y107" s="6"/>
       <c r="AE107" t="str">
         <f t="shared" si="10"/>
-        <v>10</v>
+        <v>03</v>
       </c>
       <c r="AF107" t="str">
         <f t="shared" si="11"/>
-        <v>C0</v>
+        <v>08</v>
       </c>
     </row>
     <row r="108" spans="10:35" x14ac:dyDescent="0.4">
@@ -3526,11 +3528,11 @@
       <c r="Y108" s="6"/>
       <c r="AE108" t="str">
         <f t="shared" si="10"/>
-        <v>10</v>
+        <v>1E</v>
       </c>
       <c r="AF108" t="str">
         <f t="shared" si="11"/>
-        <v>78</v>
+        <v>08</v>
       </c>
     </row>
     <row r="109" spans="10:35" x14ac:dyDescent="0.4">
@@ -3558,11 +3560,11 @@
       <c r="Y109" s="6"/>
       <c r="AE109" t="str">
         <f t="shared" si="10"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AF109" t="str">
         <f t="shared" si="11"/>
-        <v>48</v>
+        <v>08</v>
       </c>
     </row>
     <row r="110" spans="10:35" x14ac:dyDescent="0.4">
@@ -3590,11 +3592,11 @@
       <c r="Y110" s="6"/>
       <c r="AE110" t="str">
         <f t="shared" si="10"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AF110" t="str">
         <f t="shared" si="11"/>
-        <v>48</v>
+        <v>08</v>
       </c>
     </row>
     <row r="111" spans="10:35" x14ac:dyDescent="0.4">
@@ -3622,11 +3624,11 @@
       <c r="Y111" s="6"/>
       <c r="AE111" t="str">
         <f t="shared" si="10"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AF111" t="str">
         <f t="shared" si="11"/>
-        <v>48</v>
+        <v>08</v>
       </c>
     </row>
     <row r="112" spans="10:35" x14ac:dyDescent="0.4">
@@ -3658,11 +3660,11 @@
       <c r="Y112" s="6"/>
       <c r="AE112" t="str">
         <f t="shared" si="10"/>
-        <v>10</v>
+        <v>1E</v>
       </c>
       <c r="AF112" t="str">
         <f t="shared" si="11"/>
-        <v>78</v>
+        <v>08</v>
       </c>
     </row>
     <row r="113" spans="10:35" x14ac:dyDescent="0.4">
@@ -3690,11 +3692,11 @@
       <c r="Y113" s="6"/>
       <c r="AE113" t="str">
         <f t="shared" si="10"/>
-        <v>10</v>
+        <v>03</v>
       </c>
       <c r="AF113" t="str">
         <f t="shared" si="11"/>
-        <v>C0</v>
+        <v>08</v>
       </c>
     </row>
     <row r="114" spans="10:35" x14ac:dyDescent="0.4">
@@ -3722,11 +3724,11 @@
       <c r="Y114" s="6"/>
       <c r="AE114" t="str">
         <f t="shared" si="10"/>
-        <v>11</v>
+        <v>01</v>
       </c>
       <c r="AF114" t="str">
         <f t="shared" si="11"/>
-        <v>80</v>
+        <v>88</v>
       </c>
     </row>
     <row r="115" spans="10:35" x14ac:dyDescent="0.4">
@@ -3754,11 +3756,11 @@
       <c r="Y115" s="6"/>
       <c r="AE115" t="str">
         <f t="shared" si="10"/>
-        <v>13</v>
+        <v>00</v>
       </c>
       <c r="AF115" t="str">
         <f t="shared" si="11"/>
-        <v>00</v>
+        <v>C8</v>
       </c>
     </row>
     <row r="116" spans="10:35" x14ac:dyDescent="0.4">
@@ -3788,11 +3790,11 @@
       <c r="Y116" s="6"/>
       <c r="AE116" t="str">
         <f t="shared" si="10"/>
-        <v>1E</v>
+        <v>00</v>
       </c>
       <c r="AF116" t="str">
         <f t="shared" si="11"/>
-        <v>00</v>
+        <v>78</v>
       </c>
     </row>
     <row r="117" spans="10:35" x14ac:dyDescent="0.4">
@@ -3839,11 +3841,11 @@
       <c r="X120" s="3"/>
       <c r="Y120" s="4"/>
       <c r="AE120" t="str">
-        <f>DEC2HEX(R120*1+S120*2+T120*4+U120*8+V120*16+W120*32+X120*64+Y120*128, 2)</f>
+        <f>DEC2HEX(J120*128+K120*64+L120*32+M120*16+N120*8+O120*4+P120*2+Q120*1, 2)</f>
         <v>00</v>
       </c>
       <c r="AF120" t="str">
-        <f>DEC2HEX(J120*1+K120*2+L120*4+M120*8+N120*16+O120*32+P120*64+Q120*128, 2)</f>
+        <f>DEC2HEX(R120*128+S120*64+T120*32+U120*16+V120*8+W120*4+X120*2+Y120*1, 2)</f>
         <v>00</v>
       </c>
       <c r="AI120" t="str">
@@ -3869,11 +3871,11 @@
       <c r="X121" s="1"/>
       <c r="Y121" s="6"/>
       <c r="AE121" t="str">
-        <f t="shared" ref="AE121:AE135" si="12">DEC2HEX(R121*1+S121*2+T121*4+U121*8+V121*16+W121*32+X121*64+Y121*128, 2)</f>
+        <f t="shared" ref="AE121:AE135" si="12">DEC2HEX(J121*128+K121*64+L121*32+M121*16+N121*8+O121*4+P121*2+Q121*1, 2)</f>
         <v>00</v>
       </c>
       <c r="AF121" t="str">
-        <f t="shared" ref="AF121:AF135" si="13">DEC2HEX(J121*1+K121*2+L121*4+M121*8+N121*16+O121*32+P121*64+Q121*128, 2)</f>
+        <f t="shared" ref="AF121:AF135" si="13">DEC2HEX(R121*128+S121*64+T121*32+U121*16+V121*8+W121*4+X121*2+Y121*1, 2)</f>
         <v>00</v>
       </c>
       <c r="AI121" t="str">

</xml_diff>

<commit_message>
feat: Display Track Number and Year from ID3 info
</commit_message>
<xml_diff>
--- a/src/ICON16x16.xlsx
+++ b/src/ICON16x16.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Data\work\Teensy40\VSCode\Mp3FilePlayer\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{499AF711-153A-4D0E-83FC-1E0FC0EEC022}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21419BCB-58EA-4A6E-8B2E-AAF72404E3DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="150" yWindow="1065" windowWidth="28350" windowHeight="15150" xr2:uid="{7E682170-0FA3-4D33-A3CA-4458C6F2D2D4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7E682170-0FA3-4D33-A3CA-4458C6F2D2D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -20,12 +20,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -512,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94F949ED-4E88-4139-A003-24C46D6923AF}">
-  <dimension ref="J12:AI135"/>
+  <dimension ref="J12:AI153"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AI12" sqref="AI12"/>
+    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AI138" sqref="AI138:AI139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.125" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -4113,7 +4107,7 @@
         <v>08</v>
       </c>
     </row>
-    <row r="129" spans="10:32" x14ac:dyDescent="0.4">
+    <row r="129" spans="10:35" x14ac:dyDescent="0.4">
       <c r="J129" s="5"/>
       <c r="K129" s="1"/>
       <c r="L129" s="1"/>
@@ -4143,7 +4137,7 @@
         <v>08</v>
       </c>
     </row>
-    <row r="130" spans="10:32" x14ac:dyDescent="0.4">
+    <row r="130" spans="10:35" x14ac:dyDescent="0.4">
       <c r="J130" s="5"/>
       <c r="K130" s="1"/>
       <c r="L130" s="1"/>
@@ -4173,7 +4167,7 @@
         <v>08</v>
       </c>
     </row>
-    <row r="131" spans="10:32" x14ac:dyDescent="0.4">
+    <row r="131" spans="10:35" x14ac:dyDescent="0.4">
       <c r="J131" s="5"/>
       <c r="K131" s="1"/>
       <c r="L131" s="1"/>
@@ -4203,7 +4197,7 @@
         <v>08</v>
       </c>
     </row>
-    <row r="132" spans="10:32" x14ac:dyDescent="0.4">
+    <row r="132" spans="10:35" x14ac:dyDescent="0.4">
       <c r="J132" s="5"/>
       <c r="K132" s="1"/>
       <c r="L132" s="1"/>
@@ -4233,7 +4227,7 @@
         <v>08</v>
       </c>
     </row>
-    <row r="133" spans="10:32" x14ac:dyDescent="0.4">
+    <row r="133" spans="10:35" x14ac:dyDescent="0.4">
       <c r="J133" s="5"/>
       <c r="K133" s="1"/>
       <c r="L133" s="1"/>
@@ -4263,7 +4257,7 @@
         <v>08</v>
       </c>
     </row>
-    <row r="134" spans="10:32" x14ac:dyDescent="0.4">
+    <row r="134" spans="10:35" x14ac:dyDescent="0.4">
       <c r="J134" s="5"/>
       <c r="K134" s="1"/>
       <c r="L134" s="1"/>
@@ -4309,7 +4303,7 @@
         <v>F8</v>
       </c>
     </row>
-    <row r="135" spans="10:32" x14ac:dyDescent="0.4">
+    <row r="135" spans="10:35" x14ac:dyDescent="0.4">
       <c r="J135" s="7"/>
       <c r="K135" s="8"/>
       <c r="L135" s="8"/>
@@ -4335,6 +4329,576 @@
         <v>00</v>
       </c>
     </row>
+    <row r="138" spans="10:35" x14ac:dyDescent="0.4">
+      <c r="J138" s="2"/>
+      <c r="K138" s="3"/>
+      <c r="L138" s="3"/>
+      <c r="M138" s="3"/>
+      <c r="N138" s="3"/>
+      <c r="O138" s="3"/>
+      <c r="P138" s="3"/>
+      <c r="Q138" s="3"/>
+      <c r="R138" s="3"/>
+      <c r="S138" s="3"/>
+      <c r="T138" s="3"/>
+      <c r="U138" s="3"/>
+      <c r="V138" s="3"/>
+      <c r="W138" s="3"/>
+      <c r="X138" s="3"/>
+      <c r="Y138" s="4"/>
+      <c r="AE138" t="str">
+        <f>DEC2HEX(J138*128+K138*64+L138*32+M138*16+N138*8+O138*4+P138*2+Q138*1, 2)</f>
+        <v>00</v>
+      </c>
+      <c r="AF138" t="str">
+        <f>DEC2HEX(R138*128+S138*64+T138*32+U138*16+V138*8+W138*4+X138*2+Y138*1, 2)</f>
+        <v>00</v>
+      </c>
+      <c r="AI138" t="str">
+        <f>"0x"&amp;AE138&amp;",0x"&amp;AF138&amp;",0x"&amp;AE139&amp;",0x"&amp;AF139&amp;",0x"&amp;AE140&amp;",0x"&amp;AF140&amp;",0x"&amp;AE141&amp;",0x"&amp;AF141&amp;",0x"&amp;AE142&amp;",0x"&amp;AF142&amp;",0x"&amp;AE143&amp;",0x"&amp;AF143&amp;",0x"&amp;AE144&amp;",0x"&amp;AF144&amp;",0x"&amp;AE145&amp;",0x"&amp;AF145&amp;","</f>
+        <v>0x00,0x00,0x00,0x00,0x0D,0xB0,0x3F,0xFC,0x2D,0xB4,0x20,0x04,0x20,0x34,0x2A,0xB4,</v>
+      </c>
+    </row>
+    <row r="139" spans="10:35" x14ac:dyDescent="0.4">
+      <c r="J139" s="5"/>
+      <c r="K139" s="1"/>
+      <c r="L139" s="1"/>
+      <c r="M139" s="1"/>
+      <c r="N139" s="1"/>
+      <c r="O139" s="1"/>
+      <c r="P139" s="1"/>
+      <c r="Q139" s="1"/>
+      <c r="R139" s="1"/>
+      <c r="S139" s="1"/>
+      <c r="T139" s="1"/>
+      <c r="U139" s="1"/>
+      <c r="V139" s="1"/>
+      <c r="W139" s="1"/>
+      <c r="X139" s="1"/>
+      <c r="Y139" s="6"/>
+      <c r="AE139" t="str">
+        <f t="shared" ref="AE139:AE153" si="14">DEC2HEX(J139*128+K139*64+L139*32+M139*16+N139*8+O139*4+P139*2+Q139*1, 2)</f>
+        <v>00</v>
+      </c>
+      <c r="AF139" t="str">
+        <f t="shared" ref="AF139:AF153" si="15">DEC2HEX(R139*128+S139*64+T139*32+U139*16+V139*8+W139*4+X139*2+Y139*1, 2)</f>
+        <v>00</v>
+      </c>
+      <c r="AI139" t="str">
+        <f>"0x"&amp;AE146&amp;",0x"&amp;AF146&amp;",0x"&amp;AE147&amp;",0x"&amp;AF147&amp;",0x"&amp;AE148&amp;",0x"&amp;AF148&amp;",0x"&amp;AE149&amp;",0x"&amp;AF149&amp;",0x"&amp;AE150&amp;",0x"&amp;AF150&amp;",0x"&amp;AE151&amp;",0x"&amp;AF151&amp;",0x"&amp;AE152&amp;",0x"&amp;AF152&amp;",0x"&amp;AE153&amp;",0x"&amp;AF153&amp;","</f>
+        <v>0x20,0x04,0x2A,0xA4,0x20,0x04,0x2A,0xBC,0x20,0x24,0x20,0x28,0x3F,0xF0,0x00,0x00,</v>
+      </c>
+    </row>
+    <row r="140" spans="10:35" x14ac:dyDescent="0.4">
+      <c r="J140" s="5"/>
+      <c r="K140" s="1"/>
+      <c r="L140" s="1"/>
+      <c r="M140" s="1"/>
+      <c r="N140" s="10">
+        <v>1</v>
+      </c>
+      <c r="O140" s="10">
+        <v>1</v>
+      </c>
+      <c r="P140" s="1"/>
+      <c r="Q140" s="10">
+        <v>1</v>
+      </c>
+      <c r="R140" s="10">
+        <v>1</v>
+      </c>
+      <c r="S140" s="1"/>
+      <c r="T140" s="10">
+        <v>1</v>
+      </c>
+      <c r="U140" s="10">
+        <v>1</v>
+      </c>
+      <c r="V140" s="1"/>
+      <c r="W140" s="1"/>
+      <c r="X140" s="1"/>
+      <c r="Y140" s="6"/>
+      <c r="AE140" t="str">
+        <f t="shared" si="14"/>
+        <v>0D</v>
+      </c>
+      <c r="AF140" t="str">
+        <f t="shared" si="15"/>
+        <v>B0</v>
+      </c>
+    </row>
+    <row r="141" spans="10:35" x14ac:dyDescent="0.4">
+      <c r="J141" s="5"/>
+      <c r="K141" s="1"/>
+      <c r="L141" s="10">
+        <v>1</v>
+      </c>
+      <c r="M141" s="10">
+        <v>1</v>
+      </c>
+      <c r="N141" s="10">
+        <v>1</v>
+      </c>
+      <c r="O141" s="10">
+        <v>1</v>
+      </c>
+      <c r="P141" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q141" s="10">
+        <v>1</v>
+      </c>
+      <c r="R141" s="10">
+        <v>1</v>
+      </c>
+      <c r="S141" s="10">
+        <v>1</v>
+      </c>
+      <c r="T141" s="10">
+        <v>1</v>
+      </c>
+      <c r="U141" s="10">
+        <v>1</v>
+      </c>
+      <c r="V141" s="10">
+        <v>1</v>
+      </c>
+      <c r="W141" s="10">
+        <v>1</v>
+      </c>
+      <c r="X141" s="1"/>
+      <c r="Y141" s="6"/>
+      <c r="AE141" t="str">
+        <f t="shared" si="14"/>
+        <v>3F</v>
+      </c>
+      <c r="AF141" t="str">
+        <f t="shared" si="15"/>
+        <v>FC</v>
+      </c>
+    </row>
+    <row r="142" spans="10:35" x14ac:dyDescent="0.4">
+      <c r="J142" s="5"/>
+      <c r="K142" s="1"/>
+      <c r="L142" s="10">
+        <v>1</v>
+      </c>
+      <c r="M142" s="1"/>
+      <c r="N142" s="10">
+        <v>1</v>
+      </c>
+      <c r="O142" s="10">
+        <v>1</v>
+      </c>
+      <c r="P142" s="1"/>
+      <c r="Q142" s="10">
+        <v>1</v>
+      </c>
+      <c r="R142" s="10">
+        <v>1</v>
+      </c>
+      <c r="S142" s="1"/>
+      <c r="T142" s="10">
+        <v>1</v>
+      </c>
+      <c r="U142" s="10">
+        <v>1</v>
+      </c>
+      <c r="V142" s="1"/>
+      <c r="W142" s="10">
+        <v>1</v>
+      </c>
+      <c r="X142" s="1"/>
+      <c r="Y142" s="6"/>
+      <c r="AE142" t="str">
+        <f t="shared" si="14"/>
+        <v>2D</v>
+      </c>
+      <c r="AF142" t="str">
+        <f t="shared" si="15"/>
+        <v>B4</v>
+      </c>
+    </row>
+    <row r="143" spans="10:35" x14ac:dyDescent="0.4">
+      <c r="J143" s="5"/>
+      <c r="K143" s="1"/>
+      <c r="L143" s="10">
+        <v>1</v>
+      </c>
+      <c r="M143" s="1"/>
+      <c r="N143" s="1"/>
+      <c r="O143" s="1"/>
+      <c r="P143" s="1"/>
+      <c r="Q143" s="1"/>
+      <c r="R143" s="1"/>
+      <c r="S143" s="1"/>
+      <c r="T143" s="1"/>
+      <c r="U143" s="1"/>
+      <c r="V143" s="1"/>
+      <c r="W143" s="10">
+        <v>1</v>
+      </c>
+      <c r="X143" s="1"/>
+      <c r="Y143" s="6"/>
+      <c r="AE143" t="str">
+        <f t="shared" si="14"/>
+        <v>20</v>
+      </c>
+      <c r="AF143" t="str">
+        <f t="shared" si="15"/>
+        <v>04</v>
+      </c>
+    </row>
+    <row r="144" spans="10:35" x14ac:dyDescent="0.4">
+      <c r="J144" s="5"/>
+      <c r="K144" s="1"/>
+      <c r="L144" s="10">
+        <v>1</v>
+      </c>
+      <c r="M144" s="1"/>
+      <c r="N144" s="1"/>
+      <c r="O144" s="1"/>
+      <c r="P144" s="1"/>
+      <c r="Q144" s="1"/>
+      <c r="R144" s="1"/>
+      <c r="S144" s="1"/>
+      <c r="T144" s="10">
+        <v>1</v>
+      </c>
+      <c r="U144" s="10">
+        <v>1</v>
+      </c>
+      <c r="V144" s="1"/>
+      <c r="W144" s="10">
+        <v>1</v>
+      </c>
+      <c r="X144" s="1"/>
+      <c r="Y144" s="6"/>
+      <c r="AE144" t="str">
+        <f t="shared" si="14"/>
+        <v>20</v>
+      </c>
+      <c r="AF144" t="str">
+        <f t="shared" si="15"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="145" spans="10:32" x14ac:dyDescent="0.4">
+      <c r="J145" s="5"/>
+      <c r="K145" s="1"/>
+      <c r="L145" s="10">
+        <v>1</v>
+      </c>
+      <c r="M145" s="1"/>
+      <c r="N145" s="10">
+        <v>1</v>
+      </c>
+      <c r="O145" s="1"/>
+      <c r="P145" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q145" s="1"/>
+      <c r="R145" s="10">
+        <v>1</v>
+      </c>
+      <c r="S145" s="1"/>
+      <c r="T145" s="10">
+        <v>1</v>
+      </c>
+      <c r="U145" s="10">
+        <v>1</v>
+      </c>
+      <c r="V145" s="1"/>
+      <c r="W145" s="10">
+        <v>1</v>
+      </c>
+      <c r="X145" s="1"/>
+      <c r="Y145" s="6"/>
+      <c r="AE145" t="str">
+        <f t="shared" si="14"/>
+        <v>2A</v>
+      </c>
+      <c r="AF145" t="str">
+        <f t="shared" si="15"/>
+        <v>B4</v>
+      </c>
+    </row>
+    <row r="146" spans="10:32" x14ac:dyDescent="0.4">
+      <c r="J146" s="5"/>
+      <c r="K146" s="1"/>
+      <c r="L146" s="10">
+        <v>1</v>
+      </c>
+      <c r="M146" s="1"/>
+      <c r="N146" s="1"/>
+      <c r="O146" s="1"/>
+      <c r="P146" s="1"/>
+      <c r="Q146" s="1"/>
+      <c r="R146" s="1"/>
+      <c r="S146" s="1"/>
+      <c r="T146" s="1"/>
+      <c r="U146" s="1"/>
+      <c r="V146" s="1"/>
+      <c r="W146" s="10">
+        <v>1</v>
+      </c>
+      <c r="X146" s="1"/>
+      <c r="Y146" s="6"/>
+      <c r="AE146" t="str">
+        <f t="shared" si="14"/>
+        <v>20</v>
+      </c>
+      <c r="AF146" t="str">
+        <f t="shared" si="15"/>
+        <v>04</v>
+      </c>
+    </row>
+    <row r="147" spans="10:32" x14ac:dyDescent="0.4">
+      <c r="J147" s="5"/>
+      <c r="K147" s="1"/>
+      <c r="L147" s="10">
+        <v>1</v>
+      </c>
+      <c r="M147" s="1"/>
+      <c r="N147" s="10">
+        <v>1</v>
+      </c>
+      <c r="O147" s="1"/>
+      <c r="P147" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q147" s="1"/>
+      <c r="R147" s="10">
+        <v>1</v>
+      </c>
+      <c r="S147" s="1"/>
+      <c r="T147" s="10">
+        <v>1</v>
+      </c>
+      <c r="U147" s="1"/>
+      <c r="V147" s="1"/>
+      <c r="W147" s="10">
+        <v>1</v>
+      </c>
+      <c r="X147" s="1"/>
+      <c r="Y147" s="6"/>
+      <c r="AE147" t="str">
+        <f t="shared" si="14"/>
+        <v>2A</v>
+      </c>
+      <c r="AF147" t="str">
+        <f t="shared" si="15"/>
+        <v>A4</v>
+      </c>
+    </row>
+    <row r="148" spans="10:32" x14ac:dyDescent="0.4">
+      <c r="J148" s="5"/>
+      <c r="K148" s="1"/>
+      <c r="L148" s="10">
+        <v>1</v>
+      </c>
+      <c r="M148" s="1"/>
+      <c r="N148" s="1"/>
+      <c r="O148" s="1"/>
+      <c r="P148" s="1"/>
+      <c r="Q148" s="1"/>
+      <c r="R148" s="1"/>
+      <c r="S148" s="1"/>
+      <c r="T148" s="1"/>
+      <c r="U148" s="1"/>
+      <c r="V148" s="1"/>
+      <c r="W148" s="10">
+        <v>1</v>
+      </c>
+      <c r="X148" s="1"/>
+      <c r="Y148" s="6"/>
+      <c r="AE148" t="str">
+        <f t="shared" si="14"/>
+        <v>20</v>
+      </c>
+      <c r="AF148" t="str">
+        <f t="shared" si="15"/>
+        <v>04</v>
+      </c>
+    </row>
+    <row r="149" spans="10:32" x14ac:dyDescent="0.4">
+      <c r="J149" s="5"/>
+      <c r="K149" s="1"/>
+      <c r="L149" s="10">
+        <v>1</v>
+      </c>
+      <c r="M149" s="1"/>
+      <c r="N149" s="10">
+        <v>1</v>
+      </c>
+      <c r="O149" s="1"/>
+      <c r="P149" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q149" s="1"/>
+      <c r="R149" s="10">
+        <v>1</v>
+      </c>
+      <c r="S149" s="1"/>
+      <c r="T149" s="10">
+        <v>1</v>
+      </c>
+      <c r="U149" s="10">
+        <v>1</v>
+      </c>
+      <c r="V149" s="10">
+        <v>1</v>
+      </c>
+      <c r="W149" s="10">
+        <v>1</v>
+      </c>
+      <c r="X149" s="1"/>
+      <c r="Y149" s="6"/>
+      <c r="AE149" t="str">
+        <f t="shared" si="14"/>
+        <v>2A</v>
+      </c>
+      <c r="AF149" t="str">
+        <f t="shared" si="15"/>
+        <v>BC</v>
+      </c>
+    </row>
+    <row r="150" spans="10:32" x14ac:dyDescent="0.4">
+      <c r="J150" s="5"/>
+      <c r="K150" s="1"/>
+      <c r="L150" s="10">
+        <v>1</v>
+      </c>
+      <c r="M150" s="1"/>
+      <c r="N150" s="1"/>
+      <c r="O150" s="1"/>
+      <c r="P150" s="1"/>
+      <c r="Q150" s="1"/>
+      <c r="R150" s="1"/>
+      <c r="S150" s="1"/>
+      <c r="T150" s="10">
+        <v>1</v>
+      </c>
+      <c r="U150" s="1"/>
+      <c r="V150" s="1"/>
+      <c r="W150" s="10">
+        <v>1</v>
+      </c>
+      <c r="X150" s="1"/>
+      <c r="Y150" s="6"/>
+      <c r="AE150" t="str">
+        <f t="shared" si="14"/>
+        <v>20</v>
+      </c>
+      <c r="AF150" t="str">
+        <f t="shared" si="15"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="151" spans="10:32" x14ac:dyDescent="0.4">
+      <c r="J151" s="5"/>
+      <c r="K151" s="1"/>
+      <c r="L151" s="10">
+        <v>1</v>
+      </c>
+      <c r="M151" s="1"/>
+      <c r="N151" s="1"/>
+      <c r="O151" s="1"/>
+      <c r="P151" s="1"/>
+      <c r="Q151" s="1"/>
+      <c r="R151" s="1"/>
+      <c r="S151" s="1"/>
+      <c r="T151" s="10">
+        <v>1</v>
+      </c>
+      <c r="U151" s="1"/>
+      <c r="V151" s="10">
+        <v>1</v>
+      </c>
+      <c r="W151" s="1"/>
+      <c r="X151" s="1"/>
+      <c r="Y151" s="6"/>
+      <c r="AE151" t="str">
+        <f t="shared" si="14"/>
+        <v>20</v>
+      </c>
+      <c r="AF151" t="str">
+        <f t="shared" si="15"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="152" spans="10:32" x14ac:dyDescent="0.4">
+      <c r="J152" s="5"/>
+      <c r="K152" s="1"/>
+      <c r="L152" s="10">
+        <v>1</v>
+      </c>
+      <c r="M152" s="10">
+        <v>1</v>
+      </c>
+      <c r="N152" s="10">
+        <v>1</v>
+      </c>
+      <c r="O152" s="10">
+        <v>1</v>
+      </c>
+      <c r="P152" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q152" s="10">
+        <v>1</v>
+      </c>
+      <c r="R152" s="10">
+        <v>1</v>
+      </c>
+      <c r="S152" s="10">
+        <v>1</v>
+      </c>
+      <c r="T152" s="10">
+        <v>1</v>
+      </c>
+      <c r="U152" s="10">
+        <v>1</v>
+      </c>
+      <c r="V152" s="1"/>
+      <c r="W152" s="1"/>
+      <c r="X152" s="1"/>
+      <c r="Y152" s="6"/>
+      <c r="AE152" t="str">
+        <f t="shared" si="14"/>
+        <v>3F</v>
+      </c>
+      <c r="AF152" t="str">
+        <f t="shared" si="15"/>
+        <v>F0</v>
+      </c>
+    </row>
+    <row r="153" spans="10:32" x14ac:dyDescent="0.4">
+      <c r="J153" s="7"/>
+      <c r="K153" s="8"/>
+      <c r="L153" s="8"/>
+      <c r="M153" s="8"/>
+      <c r="N153" s="8"/>
+      <c r="O153" s="8"/>
+      <c r="P153" s="8"/>
+      <c r="Q153" s="8"/>
+      <c r="R153" s="8"/>
+      <c r="S153" s="8"/>
+      <c r="T153" s="8"/>
+      <c r="U153" s="8"/>
+      <c r="V153" s="8"/>
+      <c r="W153" s="8"/>
+      <c r="X153" s="8"/>
+      <c r="Y153" s="9"/>
+      <c r="AE153" t="str">
+        <f t="shared" si="14"/>
+        <v>00</v>
+      </c>
+      <c r="AF153" t="str">
+        <f t="shared" si="15"/>
+        <v>00</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4344,10 +4908,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{135F94CE-4F90-4E2C-9BA7-A72E307E0FDF}">
-  <dimension ref="J10:CS208"/>
+  <dimension ref="J10:CS226"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="J65" sqref="J65:Y80"/>
+    <sheetView topLeftCell="A164" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="J211" sqref="J211:Y226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.125" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -10361,6 +10925,370 @@
       <c r="X208" s="8"/>
       <c r="Y208" s="9"/>
     </row>
+    <row r="211" spans="10:25" x14ac:dyDescent="0.4">
+      <c r="J211" s="2"/>
+      <c r="K211" s="3"/>
+      <c r="L211" s="3"/>
+      <c r="M211" s="3"/>
+      <c r="N211" s="3"/>
+      <c r="O211" s="3"/>
+      <c r="P211" s="3"/>
+      <c r="Q211" s="3"/>
+      <c r="R211" s="3"/>
+      <c r="S211" s="3"/>
+      <c r="T211" s="3"/>
+      <c r="U211" s="3"/>
+      <c r="V211" s="3"/>
+      <c r="W211" s="3"/>
+      <c r="X211" s="3"/>
+      <c r="Y211" s="4"/>
+    </row>
+    <row r="212" spans="10:25" x14ac:dyDescent="0.4">
+      <c r="J212" s="5"/>
+      <c r="K212" s="1"/>
+      <c r="L212" s="1"/>
+      <c r="M212" s="1"/>
+      <c r="N212" s="1"/>
+      <c r="O212" s="1"/>
+      <c r="P212" s="1"/>
+      <c r="Q212" s="1"/>
+      <c r="R212" s="1"/>
+      <c r="S212" s="1"/>
+      <c r="T212" s="1"/>
+      <c r="U212" s="1"/>
+      <c r="V212" s="1"/>
+      <c r="W212" s="1"/>
+      <c r="X212" s="1"/>
+      <c r="Y212" s="6"/>
+    </row>
+    <row r="213" spans="10:25" x14ac:dyDescent="0.4">
+      <c r="J213" s="5"/>
+      <c r="K213" s="1"/>
+      <c r="L213" s="1"/>
+      <c r="M213" s="1"/>
+      <c r="N213" s="10">
+        <v>1</v>
+      </c>
+      <c r="O213" s="10">
+        <v>1</v>
+      </c>
+      <c r="P213" s="1"/>
+      <c r="Q213" s="10">
+        <v>1</v>
+      </c>
+      <c r="R213" s="10">
+        <v>1</v>
+      </c>
+      <c r="S213" s="1"/>
+      <c r="T213" s="10">
+        <v>1</v>
+      </c>
+      <c r="U213" s="10">
+        <v>1</v>
+      </c>
+      <c r="V213" s="1"/>
+      <c r="W213" s="1"/>
+      <c r="X213" s="1"/>
+      <c r="Y213" s="6"/>
+    </row>
+    <row r="214" spans="10:25" x14ac:dyDescent="0.4">
+      <c r="J214" s="5"/>
+      <c r="K214" s="1"/>
+      <c r="L214" s="10">
+        <v>1</v>
+      </c>
+      <c r="M214" s="10">
+        <v>1</v>
+      </c>
+      <c r="N214" s="10">
+        <v>1</v>
+      </c>
+      <c r="O214" s="10">
+        <v>1</v>
+      </c>
+      <c r="P214" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q214" s="10">
+        <v>1</v>
+      </c>
+      <c r="R214" s="10">
+        <v>1</v>
+      </c>
+      <c r="S214" s="10">
+        <v>1</v>
+      </c>
+      <c r="T214" s="10">
+        <v>1</v>
+      </c>
+      <c r="U214" s="10">
+        <v>1</v>
+      </c>
+      <c r="V214" s="10">
+        <v>1</v>
+      </c>
+      <c r="W214" s="10">
+        <v>1</v>
+      </c>
+      <c r="X214" s="1"/>
+      <c r="Y214" s="6"/>
+    </row>
+    <row r="215" spans="10:25" x14ac:dyDescent="0.4">
+      <c r="J215" s="5"/>
+      <c r="K215" s="1"/>
+      <c r="L215" s="10"/>
+      <c r="M215" s="1"/>
+      <c r="N215" s="10">
+        <v>1</v>
+      </c>
+      <c r="O215" s="10">
+        <v>1</v>
+      </c>
+      <c r="P215" s="1"/>
+      <c r="Q215" s="10">
+        <v>1</v>
+      </c>
+      <c r="R215" s="10">
+        <v>1</v>
+      </c>
+      <c r="S215" s="1"/>
+      <c r="T215" s="10">
+        <v>1</v>
+      </c>
+      <c r="U215" s="10">
+        <v>1</v>
+      </c>
+      <c r="V215" s="1"/>
+      <c r="W215" s="10"/>
+      <c r="X215" s="1"/>
+      <c r="Y215" s="6"/>
+    </row>
+    <row r="216" spans="10:25" x14ac:dyDescent="0.4">
+      <c r="J216" s="5"/>
+      <c r="K216" s="1"/>
+      <c r="L216" s="10"/>
+      <c r="M216" s="1"/>
+      <c r="N216" s="1"/>
+      <c r="O216" s="1"/>
+      <c r="P216" s="1"/>
+      <c r="Q216" s="1"/>
+      <c r="R216" s="1"/>
+      <c r="S216" s="1"/>
+      <c r="T216" s="1"/>
+      <c r="U216" s="1"/>
+      <c r="V216" s="1"/>
+      <c r="W216" s="10"/>
+      <c r="X216" s="1"/>
+      <c r="Y216" s="6"/>
+    </row>
+    <row r="217" spans="10:25" x14ac:dyDescent="0.4">
+      <c r="J217" s="5"/>
+      <c r="K217" s="1"/>
+      <c r="L217" s="10"/>
+      <c r="M217" s="1"/>
+      <c r="N217" s="1"/>
+      <c r="O217" s="1"/>
+      <c r="P217" s="1"/>
+      <c r="Q217" s="1"/>
+      <c r="R217" s="1"/>
+      <c r="S217" s="1"/>
+      <c r="T217" s="10">
+        <v>1</v>
+      </c>
+      <c r="U217" s="10">
+        <v>1</v>
+      </c>
+      <c r="V217" s="1"/>
+      <c r="W217" s="10"/>
+      <c r="X217" s="1"/>
+      <c r="Y217" s="6"/>
+    </row>
+    <row r="218" spans="10:25" x14ac:dyDescent="0.4">
+      <c r="J218" s="5"/>
+      <c r="K218" s="1"/>
+      <c r="L218" s="10"/>
+      <c r="M218" s="1"/>
+      <c r="N218" s="10">
+        <v>1</v>
+      </c>
+      <c r="O218" s="1"/>
+      <c r="P218" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q218" s="1"/>
+      <c r="R218" s="10">
+        <v>1</v>
+      </c>
+      <c r="S218" s="1"/>
+      <c r="T218" s="10">
+        <v>1</v>
+      </c>
+      <c r="U218" s="10">
+        <v>1</v>
+      </c>
+      <c r="V218" s="1"/>
+      <c r="W218" s="10"/>
+      <c r="X218" s="1"/>
+      <c r="Y218" s="6"/>
+    </row>
+    <row r="219" spans="10:25" x14ac:dyDescent="0.4">
+      <c r="J219" s="5"/>
+      <c r="K219" s="1"/>
+      <c r="L219" s="10"/>
+      <c r="M219" s="1"/>
+      <c r="N219" s="1"/>
+      <c r="O219" s="1"/>
+      <c r="P219" s="1"/>
+      <c r="Q219" s="1"/>
+      <c r="R219" s="1"/>
+      <c r="S219" s="1"/>
+      <c r="T219" s="1"/>
+      <c r="U219" s="1"/>
+      <c r="V219" s="1"/>
+      <c r="W219" s="10"/>
+      <c r="X219" s="1"/>
+      <c r="Y219" s="6"/>
+    </row>
+    <row r="220" spans="10:25" x14ac:dyDescent="0.4">
+      <c r="J220" s="5"/>
+      <c r="K220" s="1"/>
+      <c r="L220" s="10"/>
+      <c r="M220" s="1"/>
+      <c r="N220" s="10">
+        <v>1</v>
+      </c>
+      <c r="O220" s="1"/>
+      <c r="P220" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q220" s="1"/>
+      <c r="R220" s="10">
+        <v>1</v>
+      </c>
+      <c r="S220" s="1"/>
+      <c r="T220" s="10">
+        <v>1</v>
+      </c>
+      <c r="U220" s="1"/>
+      <c r="V220" s="1"/>
+      <c r="W220" s="10"/>
+      <c r="X220" s="1"/>
+      <c r="Y220" s="6"/>
+    </row>
+    <row r="221" spans="10:25" x14ac:dyDescent="0.4">
+      <c r="J221" s="5"/>
+      <c r="K221" s="1"/>
+      <c r="L221" s="10"/>
+      <c r="M221" s="1"/>
+      <c r="N221" s="1"/>
+      <c r="O221" s="1"/>
+      <c r="P221" s="1"/>
+      <c r="Q221" s="1"/>
+      <c r="R221" s="1"/>
+      <c r="S221" s="1"/>
+      <c r="T221" s="1"/>
+      <c r="U221" s="1"/>
+      <c r="V221" s="1"/>
+      <c r="W221" s="10"/>
+      <c r="X221" s="1"/>
+      <c r="Y221" s="6"/>
+    </row>
+    <row r="222" spans="10:25" x14ac:dyDescent="0.4">
+      <c r="J222" s="5"/>
+      <c r="K222" s="1"/>
+      <c r="L222" s="10"/>
+      <c r="M222" s="1"/>
+      <c r="N222" s="10">
+        <v>1</v>
+      </c>
+      <c r="O222" s="1"/>
+      <c r="P222" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q222" s="1"/>
+      <c r="R222" s="10">
+        <v>1</v>
+      </c>
+      <c r="S222" s="1"/>
+      <c r="T222" s="10"/>
+      <c r="U222" s="10"/>
+      <c r="V222" s="10"/>
+      <c r="W222" s="10"/>
+      <c r="X222" s="1"/>
+      <c r="Y222" s="6"/>
+    </row>
+    <row r="223" spans="10:25" x14ac:dyDescent="0.4">
+      <c r="J223" s="5"/>
+      <c r="K223" s="1"/>
+      <c r="L223" s="10"/>
+      <c r="M223" s="1"/>
+      <c r="N223" s="1"/>
+      <c r="O223" s="1"/>
+      <c r="P223" s="1"/>
+      <c r="Q223" s="1"/>
+      <c r="R223" s="1"/>
+      <c r="S223" s="1"/>
+      <c r="T223" s="10"/>
+      <c r="U223" s="1"/>
+      <c r="V223" s="1"/>
+      <c r="W223" s="10"/>
+      <c r="X223" s="1"/>
+      <c r="Y223" s="6"/>
+    </row>
+    <row r="224" spans="10:25" x14ac:dyDescent="0.4">
+      <c r="J224" s="5"/>
+      <c r="K224" s="1"/>
+      <c r="L224" s="10"/>
+      <c r="M224" s="1"/>
+      <c r="N224" s="1"/>
+      <c r="O224" s="1"/>
+      <c r="P224" s="1"/>
+      <c r="Q224" s="1"/>
+      <c r="R224" s="1"/>
+      <c r="S224" s="1"/>
+      <c r="T224" s="10"/>
+      <c r="U224" s="1"/>
+      <c r="V224" s="10"/>
+      <c r="W224" s="1"/>
+      <c r="X224" s="1"/>
+      <c r="Y224" s="6"/>
+    </row>
+    <row r="225" spans="10:25" x14ac:dyDescent="0.4">
+      <c r="J225" s="5"/>
+      <c r="K225" s="1"/>
+      <c r="L225" s="10"/>
+      <c r="M225" s="10"/>
+      <c r="N225" s="10"/>
+      <c r="O225" s="10"/>
+      <c r="P225" s="10"/>
+      <c r="Q225" s="10"/>
+      <c r="R225" s="10"/>
+      <c r="S225" s="10"/>
+      <c r="T225" s="10"/>
+      <c r="U225" s="10"/>
+      <c r="V225" s="1"/>
+      <c r="W225" s="1"/>
+      <c r="X225" s="1"/>
+      <c r="Y225" s="6"/>
+    </row>
+    <row r="226" spans="10:25" x14ac:dyDescent="0.4">
+      <c r="J226" s="7"/>
+      <c r="K226" s="8"/>
+      <c r="L226" s="8"/>
+      <c r="M226" s="8"/>
+      <c r="N226" s="8"/>
+      <c r="O226" s="8"/>
+      <c r="P226" s="8"/>
+      <c r="Q226" s="8"/>
+      <c r="R226" s="8"/>
+      <c r="S226" s="8"/>
+      <c r="T226" s="8"/>
+      <c r="U226" s="8"/>
+      <c r="V226" s="8"/>
+      <c r="W226" s="8"/>
+      <c r="X226" s="8"/>
+      <c r="Y226" s="9"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>